<commit_message>
Code, raw data, and cleaned data for 2016 charity costs.
</commit_message>
<xml_diff>
--- a/CharityCosts_17_AHA_DSHS.xlsx
+++ b/CharityCosts_17_AHA_DSHS.xlsx
@@ -451,19 +451,19 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B2">
-        <v>1130950</v>
+        <v>293105</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Parkland Memorial Hospital</t>
+          <t>University Hospital</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>DALLAS</t>
+          <t>BEXAR</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -472,54 +472,60 @@
         </is>
       </c>
       <c r="F2">
-        <v>138672432</v>
+        <v>6940900</v>
       </c>
       <c r="G2">
-        <v>1649217076</v>
+        <v>1144160290</v>
       </c>
       <c r="H2">
-        <v>2464173615</v>
+        <v>1404986559</v>
       </c>
       <c r="I2">
-        <v>3912783783</v>
+        <v>1330472170</v>
       </c>
       <c r="J2">
-        <v>6376957398</v>
+        <v>2735458729</v>
       </c>
       <c r="K2">
-        <v>831325654</v>
+        <v>136750936</v>
       </c>
       <c r="L2">
-        <v>1970410320</v>
+        <v>503605279</v>
       </c>
       <c r="M2">
-        <v>0.2531170614399376</v>
+        <v>0.4172113640553589</v>
       </c>
       <c r="N2">
-        <v>1970410320</v>
+        <v>503605279</v>
+      </c>
+      <c r="O2">
+        <v>640356215</v>
+      </c>
+      <c r="P2">
+        <v>267163889.9414766</v>
       </c>
       <c r="Q2">
-        <v>498744470.029327</v>
+        <v>210109845.3970696</v>
       </c>
       <c r="R2">
-        <v>498744470.029327</v>
+        <v>210109845.3970696</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B3">
-        <v>2015024</v>
+        <v>1130950</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Harris Health System Ben Taub Hospital</t>
+          <t>Parkland Memorial Hospital</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>HARRIS</t>
+          <t>DALLAS</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -528,48 +534,42 @@
         </is>
       </c>
       <c r="F3">
-        <v>29508381</v>
+        <v>131483015</v>
       </c>
       <c r="G3">
-        <v>1338543197</v>
+        <v>1631498659</v>
       </c>
       <c r="H3">
-        <v>973223044</v>
+        <v>2315400264</v>
       </c>
       <c r="I3">
-        <v>2118965865</v>
+        <v>3504218877</v>
       </c>
       <c r="J3">
-        <v>3092188909</v>
+        <v>5819619141</v>
       </c>
       <c r="K3">
-        <v>70638197</v>
+        <v>607674875</v>
       </c>
       <c r="L3">
-        <v>1524953518</v>
+        <v>2110198804</v>
       </c>
       <c r="M3">
-        <v>0.4287869939496921</v>
+        <v>0.2741506726371847</v>
       </c>
       <c r="N3">
-        <v>1524953518</v>
-      </c>
-      <c r="O3">
-        <v>1595591715</v>
-      </c>
-      <c r="P3">
-        <v>684168975.0458838</v>
+        <v>2110198804</v>
       </c>
       <c r="Q3">
-        <v>653880234.8962276</v>
+        <v>578512421.5147827</v>
       </c>
       <c r="R3">
-        <v>653880234.8962276</v>
+        <v>578512421.5147827</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B4">
         <v>1411240</v>
@@ -590,60 +590,60 @@
         </is>
       </c>
       <c r="F4">
-        <v>265646294</v>
+        <v>242070017</v>
       </c>
       <c r="G4">
-        <v>628645626</v>
+        <v>608801157</v>
       </c>
       <c r="H4">
-        <v>540735723</v>
+        <v>492781458</v>
       </c>
       <c r="I4">
-        <v>563527840</v>
+        <v>514102315</v>
       </c>
       <c r="J4">
-        <v>1104263563</v>
+        <v>1006883773</v>
       </c>
       <c r="K4">
-        <v>141959839</v>
+        <v>119187764</v>
       </c>
       <c r="L4">
-        <v>235580909</v>
+        <v>225165406</v>
       </c>
       <c r="M4">
-        <v>0.4588956147645268</v>
+        <v>0.4874489047348982</v>
       </c>
       <c r="N4">
-        <v>235580909</v>
+        <v>224765380</v>
       </c>
       <c r="O4">
-        <v>377540748</v>
+        <v>344353170</v>
       </c>
       <c r="P4">
-        <v>173251793.6521193</v>
+        <v>167854575.5584902</v>
       </c>
       <c r="Q4">
-        <v>108107046.062341</v>
+        <v>109756630.5388887</v>
       </c>
       <c r="R4">
-        <v>108107046.062341</v>
+        <v>109561638.3033232</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B5">
-        <v>293105</v>
+        <v>2015024</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>University Hospital</t>
+          <t>Harris Health System Ben Taub Hospital</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>BEXAR</t>
+          <t>HARRIS</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -652,43 +652,43 @@
         </is>
       </c>
       <c r="F5">
-        <v>67288716</v>
+        <v>28065601</v>
       </c>
       <c r="G5">
-        <v>1192494892</v>
+        <v>1301032626</v>
       </c>
       <c r="H5">
-        <v>1502803825</v>
+        <v>1009831942</v>
       </c>
       <c r="I5">
-        <v>1524906448</v>
+        <v>2094350203</v>
       </c>
       <c r="J5">
-        <v>3027710273</v>
+        <v>3104182145</v>
       </c>
       <c r="K5">
-        <v>151457791</v>
+        <v>115154658</v>
       </c>
       <c r="L5">
-        <v>556081161</v>
+        <v>1547833906</v>
       </c>
       <c r="M5">
-        <v>0.3852973445995526</v>
+        <v>0.4153670882711843</v>
       </c>
       <c r="N5">
-        <v>553589667</v>
+        <v>1547833905</v>
       </c>
       <c r="O5">
-        <v>707538952</v>
+        <v>1662988564</v>
       </c>
       <c r="P5">
-        <v>272612879.4063503</v>
+        <v>690750717.656958</v>
       </c>
       <c r="Q5">
-        <v>214256594.7151363</v>
+        <v>642919262.662634</v>
       </c>
       <c r="R5">
-        <v>213296628.6928506</v>
+        <v>642919262.2472669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>